<commit_message>
added version and esriFieldTypeGUID
</commit_message>
<xml_diff>
--- a/Templates/Basic_Template.xlsx
+++ b/Templates/Basic_Template.xlsx
@@ -18,8 +18,8 @@
     <sheet name="types" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Reserved">types!$A$163:$A$793</definedName>
-    <definedName name="Special">types!$A$152:$A$160</definedName>
+    <definedName name="Reserved">types!$A$164:$A$794</definedName>
+    <definedName name="Special">types!$A$153:$A$161</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="861">
   <si>
     <t>type</t>
   </si>
@@ -2605,6 +2605,15 @@
   </si>
   <si>
     <t>Applies to integer and decimal fields. Displays a custom calculator widget.</t>
+  </si>
+  <si>
+    <t>esriFieldTypeGUID</t>
+  </si>
+  <si>
+    <t>Globally Unique Identifier</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
 </sst>
 </file>
@@ -2781,39 +2790,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2951,13 +2928,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D237" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D237" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D237"/>
   <tableColumns count="4">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="label" dataDxfId="7"/>
-    <tableColumn id="4" name="hint" dataDxfId="6"/>
+    <tableColumn id="3" name="label" dataDxfId="3"/>
+    <tableColumn id="4" name="hint" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3400,7 +3377,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B234">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Label" prompt="The label will act as the question in your survey (e.g., What is your name?)." sqref="C1:C1048576"/>
@@ -3484,7 +3461,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3496,9 +3473,10 @@
     <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
     <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -3511,13 +3489,16 @@
       <c r="D1" s="13" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="13" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="12"/>
     </row>
   </sheetData>
@@ -3535,11 +3516,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:L796"/>
+  <dimension ref="A2:L797"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L796"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4596,3404 +4575,3412 @@
         <v>853</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A133" s="14" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="A134" s="14" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A134" s="19" t="s">
+    <row r="135" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="A135" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B134" s="19" t="s">
+      <c r="B135" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="C134" s="26"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C135" s="1"/>
+      <c r="C135" s="26"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C136" s="1"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C138" s="1"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C139" s="1"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C140" s="1"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C141" s="1"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="C142" s="1"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C144" s="1"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C146" s="1"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C147" s="1"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>854</v>
+        <v>254</v>
       </c>
       <c r="C148" s="1"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>281</v>
+        <v>854</v>
       </c>
       <c r="C149" s="1"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="C150" s="1"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C151" s="1"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C152" s="1"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B153" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C152" s="1"/>
-    </row>
-    <row r="154" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A154" s="14" t="s">
+      <c r="C153" s="1"/>
+    </row>
+    <row r="155" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="A155" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B155" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="24" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="24" t="s">
-        <v>55</v>
+        <v>286</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="24" t="s">
-        <v>287</v>
+        <v>55</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="24" t="s">
-        <v>114</v>
+        <v>287</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="24" t="s">
-        <v>288</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="24" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="13" x14ac:dyDescent="0.25">
-      <c r="A165" s="15" t="s">
+    <row r="166" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+      <c r="A166" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="6" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="6" t="s">
         <v>477</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>294</v>
+        <v>482</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>483</v>
+        <v>294</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>296</v>
+        <v>485</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>486</v>
+        <v>297</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>298</v>
+        <v>489</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>490</v>
+        <v>299</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>300</v>
+        <v>493</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>494</v>
+        <v>300</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>309</v>
+        <v>508</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>509</v>
+        <v>309</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>310</v>
+        <v>518</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>519</v>
+        <v>310</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>315</v>
+        <v>521</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>522</v>
+        <v>315</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>316</v>
+        <v>526</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>527</v>
+        <v>316</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>319</v>
+        <v>535</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>536</v>
+        <v>319</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>320</v>
+        <v>539</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>540</v>
+        <v>320</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>323</v>
+        <v>540</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>541</v>
+        <v>323</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>324</v>
+        <v>545</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>546</v>
+        <v>325</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>327</v>
+        <v>548</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>549</v>
+        <v>327</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>328</v>
+        <v>553</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>554</v>
+        <v>329</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>330</v>
+        <v>554</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>555</v>
+        <v>330</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>336</v>
+        <v>560</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>561</v>
+        <v>336</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>339</v>
+        <v>567</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>568</v>
+        <v>339</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>341</v>
+        <v>573</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>574</v>
+        <v>341</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>346</v>
+        <v>589</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>590</v>
+        <v>346</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>347</v>
+        <v>590</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>591</v>
+        <v>347</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>350</v>
+        <v>596</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>597</v>
+        <v>350</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>351</v>
+        <v>597</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>598</v>
+        <v>351</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="25" t="b">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="25" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>600</v>
+        <v>357</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>359</v>
+        <v>604</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>605</v>
+        <v>360</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>363</v>
+        <v>609</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>610</v>
+        <v>363</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>364</v>
+        <v>610</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>611</v>
+        <v>364</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>366</v>
+        <v>616</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>617</v>
+        <v>368</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>369</v>
+        <v>618</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>619</v>
+        <v>369</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>375</v>
+        <v>626</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>627</v>
+        <v>375</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>377</v>
+        <v>629</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>630</v>
+        <v>377</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>379</v>
+        <v>632</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>633</v>
+        <v>379</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>380</v>
+        <v>633</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>634</v>
+        <v>381</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>382</v>
+        <v>634</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>635</v>
+        <v>382</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>385</v>
+        <v>642</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>643</v>
+        <v>385</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>386</v>
+        <v>644</v>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>645</v>
+        <v>386</v>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>389</v>
+        <v>658</v>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>659</v>
+        <v>389</v>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>393</v>
+        <v>681</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>682</v>
+        <v>393</v>
       </c>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="606" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>394</v>
+        <v>684</v>
       </c>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>685</v>
+        <v>394</v>
       </c>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="609" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="610" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="611" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="612" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="613" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>399</v>
+        <v>691</v>
       </c>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>692</v>
+        <v>399</v>
       </c>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>400</v>
+        <v>692</v>
       </c>
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>693</v>
+        <v>407</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="622" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>408</v>
+        <v>695</v>
       </c>
     </row>
     <row r="623" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>696</v>
+        <v>408</v>
       </c>
     </row>
     <row r="624" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>409</v>
+        <v>696</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>697</v>
+        <v>409</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>410</v>
+        <v>710</v>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>711</v>
+        <v>410</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>414</v>
+        <v>721</v>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>722</v>
+        <v>418</v>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>423</v>
+        <v>724</v>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>725</v>
+        <v>423</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="669" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>425</v>
+        <v>736</v>
       </c>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>737</v>
+        <v>425</v>
       </c>
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>427</v>
+        <v>737</v>
       </c>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>738</v>
+        <v>427</v>
       </c>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="676" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>430</v>
+        <v>742</v>
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>743</v>
+        <v>430</v>
       </c>
     </row>
     <row r="679" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="680" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="684" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="690" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>438</v>
+        <v>756</v>
       </c>
     </row>
     <row r="693" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>757</v>
+        <v>438</v>
       </c>
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="697" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>442</v>
+        <v>760</v>
       </c>
     </row>
     <row r="698" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>761</v>
+        <v>442</v>
       </c>
     </row>
     <row r="699" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="700" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="701" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>446</v>
+        <v>763</v>
       </c>
     </row>
     <row r="702" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>764</v>
+        <v>446</v>
       </c>
     </row>
     <row r="703" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="704" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="705" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="707" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="709" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="712" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="713" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="714" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="720" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="722" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="723" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="726" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="727" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>448</v>
+        <v>788</v>
       </c>
     </row>
     <row r="728" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>789</v>
+        <v>448</v>
       </c>
     </row>
     <row r="729" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>449</v>
+        <v>789</v>
       </c>
     </row>
     <row r="730" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="731" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>790</v>
+        <v>450</v>
       </c>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>452</v>
+        <v>790</v>
       </c>
     </row>
     <row r="733" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>791</v>
+        <v>452</v>
       </c>
     </row>
     <row r="734" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="735" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="736" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>453</v>
+        <v>793</v>
       </c>
     </row>
     <row r="737" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>794</v>
+        <v>453</v>
       </c>
     </row>
     <row r="738" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="739" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="740" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="741" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="742" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="743" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="744" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="745" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="746" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="747" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="748" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="749" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="750" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="751" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="752" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A752" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="752" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A752" t="b">
+    <row r="753" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A753" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="753" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A753" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="754" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="755" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>461</v>
+        <v>810</v>
       </c>
     </row>
     <row r="756" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="757" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>811</v>
+        <v>462</v>
       </c>
     </row>
     <row r="758" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="759" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="760" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="761" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="762" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="763" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="764" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>467</v>
+        <v>817</v>
       </c>
     </row>
     <row r="765" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>818</v>
+        <v>467</v>
       </c>
     </row>
     <row r="766" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="767" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="768" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="769" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="771" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="774" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="775" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="776" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="777" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>472</v>
+        <v>829</v>
       </c>
     </row>
     <row r="778" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>830</v>
+        <v>472</v>
       </c>
     </row>
     <row r="779" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>473</v>
+        <v>830</v>
       </c>
     </row>
     <row r="780" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>831</v>
+        <v>473</v>
       </c>
     </row>
     <row r="781" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="782" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>475</v>
+        <v>832</v>
       </c>
     </row>
     <row r="783" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>833</v>
+        <v>475</v>
       </c>
     </row>
     <row r="784" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="785" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="786" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="787" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="788" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="789" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="790" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="791" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="792" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="793" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="794" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="795" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="796" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A797" t="s">
         <v>846</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A76">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:A84">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Label" prompt="The label will act as the question in your survey (e.g., What is your name?)." sqref="B76 B78:B87"/>

</xml_diff>

<commit_message>
2.5 sample and template changes
</commit_message>
<xml_diff>
--- a/Templates/Basic_Template.xlsx
+++ b/Templates/Basic_Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -18,8 +18,8 @@
     <sheet name="types" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Reserved">types!$A$164:$A$794</definedName>
-    <definedName name="Special">types!$A$153:$A$161</definedName>
+    <definedName name="Reserved">types!$A$178:$A$809</definedName>
+    <definedName name="Special">types!$A$167:$A$175</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="885">
   <si>
     <t>type</t>
   </si>
@@ -2683,6 +2683,9 @@
   </si>
   <si>
     <t>Applies to image fields. Allows user to open a canvas window to sketch on. Also supports annotation on images.</t>
+  </si>
+  <si>
+    <t>GLOBALID</t>
   </si>
 </sst>
 </file>
@@ -2859,23 +2862,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3013,13 +3000,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D237" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D237" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D237"/>
   <tableColumns count="4">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="label" dataDxfId="5"/>
-    <tableColumn id="4" name="hint" dataDxfId="4"/>
+    <tableColumn id="3" name="label" dataDxfId="3"/>
+    <tableColumn id="4" name="hint" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3462,7 +3449,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B234">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Label" prompt="The label will act as the question in your survey (e.g., What is your name?)." sqref="C1:C1048576"/>
@@ -3605,7 +3592,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:F808"/>
+  <dimension ref="A2:F809"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6759,1371 +6746,1376 @@
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>614</v>
+        <v>884</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>364</v>
+        <v>614</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>615</v>
+        <v>366</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>367</v>
+        <v>616</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>617</v>
+        <v>367</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>373</v>
+        <v>624</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>625</v>
+        <v>373</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>375</v>
+        <v>627</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>628</v>
+        <v>375</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>377</v>
+        <v>630</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>631</v>
+        <v>377</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>378</v>
+        <v>631</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>632</v>
+        <v>379</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>380</v>
+        <v>632</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>633</v>
+        <v>380</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>383</v>
+        <v>640</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>641</v>
+        <v>383</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>384</v>
+        <v>642</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>643</v>
+        <v>384</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>387</v>
+        <v>656</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>657</v>
+        <v>387</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>391</v>
+        <v>679</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>680</v>
+        <v>391</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>392</v>
+        <v>682</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>683</v>
+        <v>392</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>397</v>
+        <v>689</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>690</v>
+        <v>397</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>398</v>
+        <v>690</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>691</v>
+        <v>405</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>406</v>
+        <v>693</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>694</v>
+        <v>406</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>407</v>
+        <v>694</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>695</v>
+        <v>407</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>408</v>
+        <v>708</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>709</v>
+        <v>408</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>412</v>
+        <v>719</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>720</v>
+        <v>416</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>421</v>
+        <v>722</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>723</v>
+        <v>421</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>423</v>
+        <v>734</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>735</v>
+        <v>423</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>425</v>
+        <v>735</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>736</v>
+        <v>425</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>428</v>
+        <v>740</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690" t="s">
-        <v>741</v>
+        <v>428</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704" t="s">
-        <v>436</v>
+        <v>754</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705" t="s">
-        <v>755</v>
+        <v>436</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709" t="s">
-        <v>440</v>
+        <v>758</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710" t="s">
-        <v>759</v>
+        <v>440</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713" t="s">
-        <v>444</v>
+        <v>761</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714" t="s">
-        <v>762</v>
+        <v>444</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>446</v>
+        <v>786</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>787</v>
+        <v>446</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>447</v>
+        <v>787</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>788</v>
+        <v>448</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>450</v>
+        <v>788</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>789</v>
+        <v>450</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>451</v>
+        <v>791</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>792</v>
+        <v>451</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="764" spans="1:1">
+      <c r="A764" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="764" spans="1:1">
-      <c r="A764" t="b">
+    <row r="765" spans="1:1">
+      <c r="A765" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="765" spans="1:1">
-      <c r="A765" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>459</v>
+        <v>808</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>809</v>
+        <v>460</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776" t="s">
-        <v>465</v>
+        <v>815</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777" t="s">
-        <v>816</v>
+        <v>465</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789" t="s">
-        <v>470</v>
+        <v>827</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790" t="s">
-        <v>828</v>
+        <v>470</v>
       </c>
     </row>
     <row r="791" spans="1:1">
       <c r="A791" t="s">
-        <v>471</v>
+        <v>828</v>
       </c>
     </row>
     <row r="792" spans="1:1">
       <c r="A792" t="s">
-        <v>829</v>
+        <v>471</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794" t="s">
-        <v>473</v>
+        <v>830</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795" t="s">
-        <v>831</v>
+        <v>473</v>
       </c>
     </row>
     <row r="796" spans="1:1">
       <c r="A796" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="797" spans="1:1">
       <c r="A797" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="798" spans="1:1">
       <c r="A798" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="799" spans="1:1">
       <c r="A799" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="800" spans="1:1">
       <c r="A800" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="801" spans="1:1">
       <c r="A801" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="802" spans="1:1">
       <c r="A802" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="803" spans="1:1">
       <c r="A803" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="804" spans="1:1">
       <c r="A804" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="805" spans="1:1">
       <c r="A805" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="806" spans="1:1">
       <c r="A806" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="807" spans="1:1">
       <c r="A807" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="808" spans="1:1">
       <c r="A808" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="809" spans="1:1">
+      <c r="A809" t="s">
         <v>844</v>
       </c>
     </row>

</xml_diff>